<commit_message>
Implement complete k-means++ clustering logic
</commit_message>
<xml_diff>
--- a/casos_prueba.xlsx
+++ b/casos_prueba.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\clean_code_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865D1390-2D42-4F4E-B5ED-5A2B36CC391D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7FB490-2AEA-4E7C-AA1C-9A9AD7551337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,18 +31,6 @@
     <t>Dataset</t>
   </si>
   <si>
-    <t>k</t>
-  </si>
-  <si>
-    <t>Clusters Esperados</t>
-  </si>
-  <si>
-    <t>Centros Esperados</t>
-  </si>
-  <si>
-    <t>Mensaje de Error</t>
-  </si>
-  <si>
     <t>Datos Básicos</t>
   </si>
   <si>
@@ -82,51 +70,12 @@
     <t>Error</t>
   </si>
   <si>
-    <t>PIB_per_capita: [30000, 25000, 40000]; Esperanza_de_vida: [78, 75, 82]; Tasa_alfabetizacion: [95, 90, 98]</t>
-  </si>
-  <si>
-    <t>PIB_per_capita: [30000, 25000, 40000, 32000, 28000]; Esperanza_de_vida: [78, 75, 82, 80, 76]; Tasa_alfabetizacion: [95, 90, 98, 96, 92]</t>
-  </si>
-  <si>
-    <t>PIB_per_capita: [30000, 25000, 40000, 35000]; Esperanza_de_vida: [78, 75, 82, 79]; Tasa_alfabetizacion: [95, 90, 98, 94]</t>
-  </si>
-  <si>
-    <t>PIB_per_capita: [30000, NaN, 40000]; Esperanza_de_vida: [78, 75, 82]; Tasa_alfabetizacion: [95, 90, 98]</t>
-  </si>
-  <si>
-    <t>PIB_per_capita: [30000, 25000, 1000000]; Esperanza_de_vida: [78, 75, 82]; Tasa_alfabetizacion: [95, 90, 98]</t>
-  </si>
-  <si>
-    <t>PIB_per_capita: [30000, 30000, 40000, 40000]; Esperanza_de_vida: [78, 78, 82, 82]; Tasa_alfabetizacion: [95, 95, 98, 98]</t>
-  </si>
-  <si>
-    <t>Dataset vacío: columnas PIB_per_capita, Esperanza_de_vida, Tasa_alfabetizacion, sin filas</t>
-  </si>
-  <si>
-    <t>PIB_per_capita: [30000, 25000]; Esperanza_de_vida: [78, 75]; Tasa_alfabetizacion: [95, 90]</t>
-  </si>
-  <si>
-    <t>PIB_per_capita: [30000, 25000, 40000]; Esperanza_de_vida: [78, 75, 82]; Tasa_alfabetizacion: ['noventa y cinco', 'noventa', 'noventa y ocho']</t>
-  </si>
-  <si>
-    <t>Centro 1: [27500, 76.5, 92.5]; Centro 2: [40000, 82, 98]</t>
-  </si>
-  <si>
     <t>Agrupación según valores</t>
   </si>
   <si>
     <t>Cada registro en cluster distinto (centros iguales a los datos de entrada)</t>
   </si>
   <si>
-    <t>Centro 1: [30000, 78, 95]; Centro 2: [40000, 82, 98]</t>
-  </si>
-  <si>
-    <t>El outlier (1000000) se aísla en su propio cluster</t>
-  </si>
-  <si>
-    <t>Los duplicados se agrupan juntos (centros: [30000, 78, 95] y [40000, 82, 98])</t>
-  </si>
-  <si>
     <t>El dataset está vacío</t>
   </si>
   <si>
@@ -143,6 +92,57 @@
   </si>
   <si>
     <t>SALIDAS</t>
+  </si>
+  <si>
+    <t>Expected Clusters</t>
+  </si>
+  <si>
+    <t>Number of Centroids</t>
+  </si>
+  <si>
+    <t>Expected Centers</t>
+  </si>
+  <si>
+    <t>Error Message</t>
+  </si>
+  <si>
+    <t>GDP: [30000, 25000, 40000]; Life Expectancy: [78, 75, 82]; Literacy Rate: [95, 90, 98]</t>
+  </si>
+  <si>
+    <t>GDP: [30000, 25000, 40000, 32000, 28000]; Life Expectancy: [78, 75, 82, 80, 76]; Literacy Rate: [95, 90, 98, 96, 92]</t>
+  </si>
+  <si>
+    <t>GDP: [30000, 25000, 40000, 35000]; Life Expectancy: [78, 75, 82, 79]; Literacy Rate: [95, 90, 98, 94]</t>
+  </si>
+  <si>
+    <t>GDP: [30000, NaN, 40000]; Life Expectancy: [78, 75, 82]; Literacy Rate: [95, 90, 98]</t>
+  </si>
+  <si>
+    <t>GDP: [30000, 25000, 1000000]; Life Expectancy: [78, 75, 82]; Literacy Rate: [95, 90, 98]</t>
+  </si>
+  <si>
+    <t>GDP: [30000, 30000, 40000, 40000]; Life Expectancy: [78, 78, 82, 82]; Literacy Rate: [95, 95, 98, 98]</t>
+  </si>
+  <si>
+    <t>Empty dataset: columnas: GDP, Life Expectancy, Literacy Rate, sin filas</t>
+  </si>
+  <si>
+    <t>GDP: [30000, 25000]; Life Expectancy: [78, 75]; Literacy Rate: [95, 90]</t>
+  </si>
+  <si>
+    <t>GDP: [30000, 25000, 40000]; Life Expectancy: [78, 75, 82]; Literacy Rate: ['noventa y cinco', 'noventa', 'noventa y ocho']</t>
+  </si>
+  <si>
+    <t>Centro 1: [0.16667, 0.21429, 0.31250]; Centro 2: [1.0,  1.0, 1.0]</t>
+  </si>
+  <si>
+    <t>Centro 1: [0.0, 0.0 0.0]; Centro 2: [1.0, 1.0, 1.0]</t>
+  </si>
+  <si>
+    <t>El outlier (1.0) se aísla en su propio cluster</t>
+  </si>
+  <si>
+    <t>Los duplicados se agrupan juntos (centros: [0.0, 0.0, 0.0] y [1.0, 1.0, 1.0])</t>
   </si>
 </sst>
 </file>
@@ -222,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -230,13 +230,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -552,6 +551,7 @@
     <col min="1" max="1" width="24.109375" customWidth="1"/>
     <col min="2" max="2" width="14.5546875" customWidth="1"/>
     <col min="3" max="3" width="121.6640625" customWidth="1"/>
+    <col min="4" max="4" width="31.44140625" customWidth="1"/>
     <col min="5" max="5" width="21.5546875" customWidth="1"/>
     <col min="6" max="6" width="67" customWidth="1"/>
     <col min="7" max="7" width="51.5546875" customWidth="1"/>
@@ -559,14 +559,14 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C1" s="2" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="D1" s="2"/>
-      <c r="E1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="E1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -579,204 +579,204 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4">
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5">
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7">
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8">
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="G9" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D11">
         <v>3</v>
       </c>
       <c r="G11" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D12">
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feature: Add test for errors and CLI
</commit_message>
<xml_diff>
--- a/casos_prueba.xlsx
+++ b/casos_prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\clean_code_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7FB490-2AEA-4E7C-AA1C-9A9AD7551337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCAB1A7C-8CD9-4FE4-8AD6-B7E581BDAB77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>Nombre Caso</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>Los duplicados se agrupan juntos (centros: [0.0, 0.0, 0.0] y [1.0, 1.0, 1.0])</t>
+  </si>
+  <si>
+    <t>Number of iterations</t>
   </si>
 </sst>
 </file>
@@ -233,9 +236,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -553,22 +554,24 @@
     <col min="3" max="3" width="121.6640625" customWidth="1"/>
     <col min="4" max="4" width="31.44140625" customWidth="1"/>
     <col min="5" max="5" width="21.5546875" customWidth="1"/>
-    <col min="6" max="6" width="67" customWidth="1"/>
-    <col min="7" max="7" width="51.5546875" customWidth="1"/>
+    <col min="6" max="6" width="18.21875" customWidth="1"/>
+    <col min="7" max="7" width="64.33203125" customWidth="1"/>
+    <col min="8" max="8" width="49.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C1" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D1" s="2"/>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -581,17 +584,20 @@
       <c r="D2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -605,13 +611,16 @@
         <v>2</v>
       </c>
       <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -625,13 +634,16 @@
         <v>3</v>
       </c>
       <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -645,13 +657,16 @@
         <v>4</v>
       </c>
       <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5">
         <v>4</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -665,13 +680,16 @@
         <v>2</v>
       </c>
       <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -685,13 +703,16 @@
         <v>2</v>
       </c>
       <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -705,13 +726,16 @@
         <v>2</v>
       </c>
       <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -724,11 +748,14 @@
       <c r="D9">
         <v>2</v>
       </c>
-      <c r="G9" t="s">
+      <c r="E9">
+        <v>10</v>
+      </c>
+      <c r="H9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -741,11 +768,14 @@
       <c r="D10">
         <v>0</v>
       </c>
-      <c r="G10" t="s">
+      <c r="E10">
+        <v>10</v>
+      </c>
+      <c r="H10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -758,11 +788,14 @@
       <c r="D11">
         <v>3</v>
       </c>
-      <c r="G11" t="s">
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="H11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -775,14 +808,17 @@
       <c r="D12">
         <v>2</v>
       </c>
-      <c r="G12" t="s">
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="H12" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="C1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Obtener datos del archivo
</commit_message>
<xml_diff>
--- a/casos_prueba.xlsx
+++ b/casos_prueba.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\clean_code_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codigo Limpio\machine_learning-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCAB1A7C-8CD9-4FE4-8AD6-B7E581BDAB77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55052B0F-5F4D-41E7-841A-28CEDE0BACED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>Nombre Caso</t>
   </si>
@@ -146,13 +146,16 @@
   </si>
   <si>
     <t>Number of iterations</t>
+  </si>
+  <si>
+    <t>Id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,6 +165,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -225,18 +236,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,284 +554,320 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.109375" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
-    <col min="3" max="3" width="121.6640625" customWidth="1"/>
-    <col min="4" max="4" width="31.44140625" customWidth="1"/>
-    <col min="5" max="5" width="21.5546875" customWidth="1"/>
-    <col min="6" max="6" width="18.21875" customWidth="1"/>
-    <col min="7" max="7" width="64.33203125" customWidth="1"/>
-    <col min="8" max="8" width="49.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="121.7109375" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="64.28515625" customWidth="1"/>
+    <col min="9" max="9" width="49.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C1" s="2" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="3"/>
       <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>28</v>
       </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
       <c r="E3">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>29</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>3</v>
       </c>
-      <c r="E4">
-        <v>10</v>
-      </c>
       <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4">
         <v>3</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>30</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>4</v>
       </c>
-      <c r="E5">
-        <v>10</v>
-      </c>
       <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5">
         <v>4</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>31</v>
       </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
       <c r="E6">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F6">
-        <v>2</v>
-      </c>
-      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>32</v>
       </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
       <c r="E7">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F7">
-        <v>2</v>
-      </c>
-      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>33</v>
       </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
       <c r="E8">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F8">
-        <v>2</v>
-      </c>
-      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>34</v>
       </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
       <c r="E9">
-        <v>10</v>
-      </c>
-      <c r="H9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
+      </c>
+      <c r="I9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>10</v>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
         <v>15</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>28</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>0</v>
       </c>
-      <c r="E10">
-        <v>10</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="F10">
+        <v>10</v>
+      </c>
+      <c r="I10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>15</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>35</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>3</v>
       </c>
-      <c r="E11">
-        <v>10</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="I11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>15</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>36</v>
       </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
       <c r="E12">
-        <v>10</v>
-      </c>
-      <c r="H12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="I12" t="s">
         <v>21</v>
       </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="D1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>